<commit_message>
Changes to be committed: 	modified:   LAB/Assignments/rmcmilan1MoEPoFSModule2.xlsx
</commit_message>
<xml_diff>
--- a/LAB/Assignments/rmcmilan1MoEPoFSModule2.xlsx
+++ b/LAB/Assignments/rmcmilan1MoEPoFSModule2.xlsx
@@ -305,8 +305,39 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -315,37 +346,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>33.333333333333336</c:v>
+                  <c:v>333.33333333333331</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16.666666666666668</c:v>
+                  <c:v>166.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14.285714285714285</c:v>
+                  <c:v>142.85714285714286</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.5</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11.111111111111111</c:v>
+                  <c:v>111.1111111111111</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.0909090909090917</c:v>
+                  <c:v>90.909090909090921</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.3333333333333339</c:v>
+                  <c:v>83.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.6923076923076916</c:v>
+                  <c:v>76.92307692307692</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -357,37 +388,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>3548387096774193.5</c:v>
+                  <c:v>3.5483870967741936E-9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2748387096774193.5</c:v>
+                  <c:v>2.7483870967741935E-9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2329032258064516</c:v>
+                  <c:v>2.3290322580645164E-9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1987096774193548.5</c:v>
+                  <c:v>1.9870967741935482E-9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1770967741935484</c:v>
+                  <c:v>1.7709677419354839E-9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1600000000000000</c:v>
+                  <c:v>1.6000000000000001E-9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1470967741935484</c:v>
+                  <c:v>1.4709677419354839E-9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1364516129032258</c:v>
+                  <c:v>1.3645161290322581E-9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1283870967741935.5</c:v>
+                  <c:v>1.2838709677419353E-9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1209677419354838.7</c:v>
+                  <c:v>1.2096774193548386E-9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1148387096774193.5</c:v>
+                  <c:v>1.1483870967741934E-9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -402,11 +433,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="653748808"/>
-        <c:axId val="650223008"/>
+        <c:axId val="732048224"/>
+        <c:axId val="732048616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="653748808"/>
+        <c:axId val="732048224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -519,12 +550,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="650223008"/>
+        <c:crossAx val="732048616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="650223008"/>
+        <c:axId val="732048616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -637,7 +668,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="653748808"/>
+        <c:crossAx val="732048224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -787,6 +818,65 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$B$2:$B$12</c:f>
@@ -794,37 +884,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>110000000000000</c:v>
+                  <c:v>1.0999999999999999E-10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>85200000000000</c:v>
+                  <c:v>8.52E-11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>72200000000000</c:v>
+                  <c:v>7.2200000000000007E-11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>61600000000000</c:v>
+                  <c:v>6.1599999999999999E-11</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>54900000000000</c:v>
+                  <c:v>5.4899999999999999E-11</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>49600000000000</c:v>
+                  <c:v>4.9600000000000002E-11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>45600000000000</c:v>
+                  <c:v>4.5600000000000003E-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>42300000000000</c:v>
+                  <c:v>4.2299999999999999E-11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>39800000000000</c:v>
+                  <c:v>3.9799999999999994E-11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>37500000000000</c:v>
+                  <c:v>3.75E-11</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>35600000000000</c:v>
+                  <c:v>3.5599999999999999E-11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -836,37 +926,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.03</c:v>
+                  <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.04</c:v>
+                  <c:v>4.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.05</c:v>
+                  <c:v>5.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.06</c:v>
+                  <c:v>6.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>7.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.08</c:v>
+                  <c:v>8.0000000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.09</c:v>
+                  <c:v>9.0000000000000011E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.1</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.11</c:v>
+                  <c:v>1.0999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.12</c:v>
+                  <c:v>1.2E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.13</c:v>
+                  <c:v>1.3000000000000001E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -881,11 +971,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="653749984"/>
-        <c:axId val="653191984"/>
+        <c:axId val="516504936"/>
+        <c:axId val="516505328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="653749984"/>
+        <c:axId val="516504936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -998,12 +1088,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="653191984"/>
+        <c:crossAx val="516505328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="653191984"/>
+        <c:axId val="516505328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1116,7 +1206,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="653749984"/>
+        <c:crossAx val="516504936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2282,15 +2372,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>781050</xdr:colOff>
+      <xdr:colOff>628650</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
+      <xdr:colOff>438150</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2608,7 +2698,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D40" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2639,201 +2729,201 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2">
-        <f>110*10^12</f>
-        <v>110000000000000</v>
+        <f>110*10^-12</f>
+        <v>1.0999999999999999E-10</v>
       </c>
       <c r="C2">
-        <f>3*10^-2</f>
-        <v>0.03</v>
+        <f>3*10^-3</f>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="D2">
         <f>1/(C2*10^0)</f>
-        <v>33.333333333333336</v>
+        <v>333.33333333333331</v>
       </c>
       <c r="E2">
         <f>B2/0.031</f>
-        <v>3548387096774193.5</v>
+        <v>3.5483870967741936E-9</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3">
-        <f>85.2*10^12</f>
-        <v>85200000000000</v>
+        <f>85.2*10^-12</f>
+        <v>8.52E-11</v>
       </c>
       <c r="C3">
-        <f>4*10^-2</f>
-        <v>0.04</v>
+        <f>4*10^-3</f>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D3">
         <f>1/(C3*10^0)</f>
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E12" si="0">B3/0.031</f>
-        <v>2748387096774193.5</v>
+        <v>2.7483870967741935E-9</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4">
-        <f>72.2*10^12</f>
-        <v>72200000000000</v>
+        <f>72.2*10^-12</f>
+        <v>7.2200000000000007E-11</v>
       </c>
       <c r="C4">
-        <f>5*10^-2</f>
-        <v>0.05</v>
+        <f>5*10^-3</f>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D3:D12" si="1">1/(C4*10^0)</f>
-        <v>20</v>
+        <f t="shared" ref="D4:D12" si="1">1/(C4*10^0)</f>
+        <v>200</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>2329032258064516</v>
+        <v>2.3290322580645164E-9</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5">
-        <f>61.6*10^12</f>
-        <v>61600000000000</v>
+        <f>61.6*10^-12</f>
+        <v>6.1599999999999999E-11</v>
       </c>
       <c r="C5">
-        <f>6*10^-2</f>
-        <v>0.06</v>
+        <f>6*10^-3</f>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="D5">
         <f t="shared" si="1"/>
-        <v>16.666666666666668</v>
+        <v>166.66666666666666</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>1987096774193548.5</v>
+        <v>1.9870967741935482E-9</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6">
-        <f>54.9*10^12</f>
-        <v>54900000000000</v>
+        <f>54.9*10^-12</f>
+        <v>5.4899999999999999E-11</v>
       </c>
       <c r="C6">
-        <f>7*10^-2</f>
-        <v>7.0000000000000007E-2</v>
+        <f>7*10^-3</f>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
-        <v>14.285714285714285</v>
+        <v>142.85714285714286</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>1770967741935484</v>
+        <v>1.7709677419354839E-9</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7">
-        <f>49.6*10^12</f>
-        <v>49600000000000</v>
+        <f>49.6*10^-12</f>
+        <v>4.9600000000000002E-11</v>
       </c>
       <c r="C7">
-        <f>8*10^-2</f>
-        <v>0.08</v>
+        <f>8*10^-3</f>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="D7">
         <f t="shared" si="1"/>
-        <v>12.5</v>
+        <v>125</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>1600000000000000</v>
+        <v>1.6000000000000001E-9</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8">
-        <f>45.6*10^12</f>
-        <v>45600000000000</v>
+        <f>45.6*10^-12</f>
+        <v>4.5600000000000003E-11</v>
       </c>
       <c r="C8">
-        <f>9*10^-2</f>
-        <v>0.09</v>
+        <f>9*10^-3</f>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="D8">
         <f t="shared" si="1"/>
-        <v>11.111111111111111</v>
+        <v>111.1111111111111</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>1470967741935484</v>
+        <v>1.4709677419354839E-9</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9">
-        <f>42.3*10^12</f>
-        <v>42300000000000</v>
+        <f>42.3*10^-12</f>
+        <v>4.2299999999999999E-11</v>
       </c>
       <c r="C9">
-        <f>10*10^-2</f>
-        <v>0.1</v>
+        <f>10*10^-3</f>
+        <v>0.01</v>
       </c>
       <c r="D9">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>1364516129032258</v>
+        <v>1.3645161290322581E-9</v>
       </c>
       <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10">
-        <f>39.8*10^12</f>
-        <v>39800000000000</v>
+        <f>39.8*10^-12</f>
+        <v>3.9799999999999994E-11</v>
       </c>
       <c r="C10">
-        <f>11*10^-2</f>
-        <v>0.11</v>
+        <f>11*10^-3</f>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="D10">
         <f t="shared" si="1"/>
-        <v>9.0909090909090917</v>
+        <v>90.909090909090921</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>1283870967741935.5</v>
+        <v>1.2838709677419353E-9</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11">
-        <f>37.5*10^12</f>
-        <v>37500000000000</v>
+        <f>37.5*10^-12</f>
+        <v>3.75E-11</v>
       </c>
       <c r="C11">
-        <f>12*10^-2</f>
-        <v>0.12</v>
+        <f>12*10^-3</f>
+        <v>1.2E-2</v>
       </c>
       <c r="D11">
         <f t="shared" si="1"/>
-        <v>8.3333333333333339</v>
+        <v>83.333333333333329</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>1209677419354838.7</v>
+        <v>1.2096774193548386E-9</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12">
-        <f>35.6*10^12</f>
-        <v>35600000000000</v>
+        <f>35.6*10^-12</f>
+        <v>3.5599999999999999E-11</v>
       </c>
       <c r="C12">
-        <f>13*10^-2</f>
-        <v>0.13</v>
+        <f>13*10^-3</f>
+        <v>1.3000000000000001E-2</v>
       </c>
       <c r="D12">
         <f t="shared" si="1"/>
-        <v>7.6923076923076916</v>
+        <v>76.92307692307692</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>1148387096774193.5</v>
+        <v>1.1483870967741934E-9</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2842,14 +2932,14 @@
       </c>
       <c r="B15" s="4">
         <f>$B$18</f>
-        <v>93414143016279.531</v>
+        <v>9.341414301627952E-12</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D15">
         <f>ROUND((B15-B16)/(B16),2)</f>
-        <v>1.0550278982845001E+25</v>
+        <v>0.06</v>
       </c>
       <c r="E15" t="s">
         <v>15</v>
@@ -2868,7 +2958,7 @@
       </c>
       <c r="D16">
         <f>(B15-B16)/B19</f>
-        <v>203.95408883401618</v>
+        <v>10.637789648326317</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2886,10 +2976,10 @@
       </c>
       <c r="B18">
         <f t="array" ref="B18:C22">LINEST(E2:E12,D2:D12,TRUE,TRUE)</f>
-        <v>93414143016279.531</v>
+        <v>9.341414301627952E-12</v>
       </c>
       <c r="C18">
-        <v>433314984884209.5</v>
+        <v>4.3331498488421002E-10</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>3</v>
@@ -2901,10 +2991,10 @@
         <v>2</v>
       </c>
       <c r="B19">
-        <v>458015544333.13031</v>
+        <v>4.5801554433313156E-14</v>
       </c>
       <c r="C19">
-        <v>7822841604221.9492</v>
+        <v>7.822841604221971E-12</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>8</v>
@@ -2916,10 +3006,10 @@
         <v>4</v>
       </c>
       <c r="B20">
-        <v>0.99978368645101257</v>
+        <v>0.99978368645101245</v>
       </c>
       <c r="C20">
-        <v>11611495526921.32</v>
+        <v>1.1611495526921355E-11</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>7</v>
@@ -2931,7 +3021,7 @@
         <v>6</v>
       </c>
       <c r="B21">
-        <v>41597.270352113745</v>
+        <v>41597.270352113504</v>
       </c>
       <c r="C21">
         <v>9</v>
@@ -2942,10 +3032,10 @@
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22">
-        <v>5.6084280304962206E+30</v>
+        <v>5.608428030496222E-18</v>
       </c>
       <c r="C22">
-        <v>1.2134414553454245E+27</v>
+        <v>1.2134414553454318E-21</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>

</xml_diff>